<commit_message>
Q4 third GDP revision
</commit_message>
<xml_diff>
--- a/data/raw/haver/economic_statistics.xlsx
+++ b/data/raw/haver/economic_statistics.xlsx
@@ -5701,13 +5701,13 @@
         <v>1</v>
       </c>
       <c r="F205">
-        <v>4938.666666666667</v>
+        <v>4935.333333333333</v>
       </c>
       <c r="G205">
-        <v>13656</v>
+        <v>13655.33333333333</v>
       </c>
       <c r="H205">
-        <v>325241.6666666667</v>
+        <v>327589.6666666667</v>
       </c>
     </row>
     <row r="206">
@@ -5727,13 +5727,13 @@
         <v>1</v>
       </c>
       <c r="F206">
-        <v>5008.111111111111</v>
+        <v>5007</v>
       </c>
       <c r="G206">
-        <v>13654.11111111111</v>
+        <v>13653.88888888889</v>
       </c>
       <c r="H206">
-        <v>323736.6666666667</v>
+        <v>324519.3333333333</v>
       </c>
     </row>
     <row r="207">
@@ -5753,13 +5753,13 @@
         <v>1</v>
       </c>
       <c r="F207">
-        <v>4994.37037037037</v>
+        <v>4992.888888888889</v>
       </c>
       <c r="G207">
-        <v>13682.25925925926</v>
+        <v>13681.96296296296</v>
       </c>
       <c r="H207">
-        <v>322655.5555555556</v>
+        <v>323699.1111111111</v>
       </c>
     </row>
     <row r="208">
@@ -5779,13 +5779,13 @@
         <v>1</v>
       </c>
       <c r="F208">
-        <v>4980.382716049383</v>
+        <v>4978.407407407407</v>
       </c>
       <c r="G208">
-        <v>13664.12345679012</v>
+        <v>13663.72839506173</v>
       </c>
       <c r="H208">
-        <v>323877.962962963</v>
+        <v>325269.3703703704</v>
       </c>
     </row>
     <row r="209">
@@ -5805,13 +5805,13 @@
         <v>1</v>
       </c>
       <c r="F209">
-        <v>4994.288065843622</v>
+        <v>4992.765432098765</v>
       </c>
       <c r="G209">
-        <v>13666.83127572016</v>
+        <v>13666.52674897119</v>
       </c>
       <c r="H209">
-        <v>323423.3950617284</v>
+        <v>324495.9382716049</v>
       </c>
     </row>
     <row r="210">
@@ -5831,13 +5831,13 @@
         <v>1</v>
       </c>
       <c r="F210">
-        <v>4989.680384087792</v>
+        <v>4988.020576131687</v>
       </c>
       <c r="G210">
-        <v>13671.07133058985</v>
+        <v>13670.73936899863</v>
       </c>
       <c r="H210">
-        <v>323318.9711934156</v>
+        <v>324488.1399176955</v>
       </c>
     </row>
     <row r="211">
@@ -5857,13 +5857,13 @@
         <v>1</v>
       </c>
       <c r="F211">
-        <v>4988.117055326932</v>
+        <v>4986.39780521262</v>
       </c>
       <c r="G211">
-        <v>13667.34202103338</v>
+        <v>13666.99817101052</v>
       </c>
       <c r="H211">
-        <v>323540.109739369</v>
+        <v>324751.1495198903</v>
       </c>
     </row>
     <row r="212">
@@ -5883,13 +5883,13 @@
         <v>1</v>
       </c>
       <c r="F212">
-        <v>4990.695168419448</v>
+        <v>4989.061271147691</v>
       </c>
       <c r="G212">
-        <v>13668.41487578113</v>
+        <v>13668.08809632678</v>
       </c>
       <c r="H212">
-        <v>323427.491998171</v>
+        <v>324578.4092363969</v>
       </c>
     </row>
     <row r="213">
@@ -5909,13 +5909,13 @@
         <v>1</v>
       </c>
       <c r="F213">
-        <v>4989.497535944724</v>
+        <v>4987.826550830666</v>
       </c>
       <c r="G213">
-        <v>13668.94274246812</v>
+        <v>13668.60854544531</v>
       </c>
       <c r="H213">
-        <v>323428.8576436519</v>
+        <v>324605.8995579942</v>
       </c>
     </row>
     <row r="214">
@@ -5935,13 +5935,13 @@
         <v>1</v>
       </c>
       <c r="F214">
-        <v>4989.436586563702</v>
+        <v>4987.761875730325</v>
       </c>
       <c r="G214">
-        <v>13668.23321309421</v>
+        <v>13667.89827092754</v>
       </c>
       <c r="H214">
-        <v>323465.4864603973</v>
+        <v>324645.1527714271</v>
       </c>
     </row>
     <row r="215">
@@ -5961,13 +5961,13 @@
         <v>1</v>
       </c>
       <c r="F215">
-        <v>4989.876430309291</v>
+        <v>4988.216565902894</v>
       </c>
       <c r="G215">
-        <v>13668.53027711449</v>
+        <v>13668.19830423321</v>
       </c>
       <c r="H215">
-        <v>323440.6120340734</v>
+        <v>324609.8205219394</v>
       </c>
     </row>
     <row r="216">
@@ -5987,13 +5987,13 @@
         <v>1</v>
       </c>
       <c r="F216">
-        <v>4989.603517605906</v>
+        <v>4987.934997487962</v>
       </c>
       <c r="G216">
-        <v>13668.56874422561</v>
+        <v>13668.23504020202</v>
       </c>
       <c r="H216">
-        <v>323444.9853793742</v>
+        <v>324620.2909504536</v>
       </c>
     </row>
     <row r="217">
@@ -6013,13 +6013,13 @@
         <v>1</v>
       </c>
       <c r="F217">
-        <v>4989.6388448263</v>
+        <v>4987.971146373727</v>
       </c>
       <c r="G217">
-        <v>13668.44407814477</v>
+        <v>13668.11053845425</v>
       </c>
       <c r="H217">
-        <v>323450.3612912817</v>
+        <v>324625.0880812734</v>
       </c>
     </row>
     <row r="218">
@@ -6039,13 +6039,13 @@
         <v>1</v>
       </c>
       <c r="F218">
-        <v>4989.706264247166</v>
+        <v>4988.040903254861</v>
       </c>
       <c r="G218">
-        <v>13668.51436649495</v>
+        <v>13668.18129429649</v>
       </c>
       <c r="H218">
-        <v>323445.3195682431</v>
+        <v>324618.3998512221</v>
       </c>
     </row>
     <row r="219">
@@ -6065,13 +6065,13 @@
         <v>1</v>
       </c>
       <c r="F219">
-        <v>4989.649542226457</v>
+        <v>4987.98234903885</v>
       </c>
       <c r="G219">
-        <v>13668.50906295511</v>
+        <v>13668.17562431759</v>
       </c>
       <c r="H219">
-        <v>323446.8887462996</v>
+        <v>324621.2596276497</v>
       </c>
     </row>
     <row r="220">
@@ -6091,13 +6091,13 @@
         <v>1</v>
       </c>
       <c r="F220">
-        <v>4989.664883766641</v>
+        <v>4987.998132889145</v>
       </c>
       <c r="G220">
-        <v>13668.48916919828</v>
+        <v>13668.15581902278</v>
       </c>
       <c r="H220">
-        <v>323447.5232019415</v>
+        <v>324621.5825200484</v>
       </c>
     </row>
     <row r="221">
@@ -6117,13 +6117,13 @@
         <v>1</v>
       </c>
       <c r="F221">
-        <v>4989.673563413421</v>
+        <v>4988.007128394285</v>
       </c>
       <c r="G221">
-        <v>13668.50419954945</v>
+        <v>13668.17091254562</v>
       </c>
       <c r="H221">
-        <v>323446.5771721614</v>
+        <v>324620.41399964</v>
       </c>
     </row>
     <row r="222">
@@ -6143,13 +6143,13 @@
         <v>1</v>
       </c>
       <c r="F222">
-        <v>4989.662663135507</v>
+        <v>4987.995870107427</v>
       </c>
       <c r="G222">
-        <v>13668.50081056761</v>
+        <v>13668.16745196199</v>
       </c>
       <c r="H222">
-        <v>323446.9963734675</v>
+        <v>324621.085382446</v>
       </c>
     </row>
     <row r="223">
@@ -6169,13 +6169,13 @@
         <v>1</v>
       </c>
       <c r="F223">
-        <v>4989.667036771856</v>
+        <v>4988.000377130285</v>
       </c>
       <c r="G223">
-        <v>13668.49805977178</v>
+        <v>13668.16472784346</v>
       </c>
       <c r="H223">
-        <v>323447.0322491901</v>
+        <v>324621.0273007115</v>
       </c>
     </row>
     <row r="224">
@@ -6195,13 +6195,13 @@
         <v>1</v>
       </c>
       <c r="F224">
-        <v>4989.667754440261</v>
+        <v>4988.001125210666</v>
       </c>
       <c r="G224">
-        <v>13668.50102329628</v>
+        <v>13668.16769745036</v>
       </c>
       <c r="H224">
-        <v>323446.868598273</v>
+        <v>324620.8422275992</v>
       </c>
     </row>
     <row r="225">
@@ -6221,13 +6221,13 @@
         <v>1</v>
       </c>
       <c r="F225">
-        <v>4989.665818115875</v>
+        <v>4987.999124149459</v>
       </c>
       <c r="G225">
-        <v>13668.49996454522</v>
+        <v>13668.16662575194</v>
       </c>
       <c r="H225">
-        <v>323446.9657403102</v>
+        <v>324620.9849702522</v>
       </c>
     </row>
     <row r="226">
@@ -6247,13 +6247,13 @@
         <v>1</v>
       </c>
       <c r="F226">
-        <v>4989.666869775997</v>
+        <v>4988.000208830137</v>
       </c>
       <c r="G226">
-        <v>13668.49968253776</v>
+        <v>13668.16635034859</v>
       </c>
       <c r="H226">
-        <v>323446.9555292578</v>
+        <v>324620.951499521</v>
       </c>
     </row>
     <row r="227">
@@ -6273,13 +6273,13 @@
         <v>1</v>
       </c>
       <c r="F227">
-        <v>4989.666814110711</v>
+        <v>4988.000152730087</v>
       </c>
       <c r="G227">
-        <v>13668.50022345975</v>
+        <v>13668.16689118363</v>
       </c>
       <c r="H227">
-        <v>323446.929955947</v>
+        <v>324620.9262324575</v>
       </c>
     </row>
     <row r="228">
@@ -6299,13 +6299,13 @@
         <v>1</v>
       </c>
       <c r="F228">
-        <v>4989.666500667528</v>
+        <v>4987.999828569895</v>
       </c>
       <c r="G228">
-        <v>13668.49995684758</v>
+        <v>13668.16662242805</v>
       </c>
       <c r="H228">
-        <v>323446.950408505</v>
+        <v>324620.9542340769</v>
       </c>
     </row>
     <row r="229">
@@ -6325,13 +6325,13 @@
         <v>1</v>
       </c>
       <c r="F229">
-        <v>4989.666728184745</v>
+        <v>4988.000063376707</v>
       </c>
       <c r="G229">
-        <v>13668.4999542817</v>
+        <v>13668.16662132009</v>
       </c>
       <c r="H229">
-        <v>323446.9452979033</v>
+        <v>324620.9439886851</v>
       </c>
     </row>
     <row r="230">
@@ -6351,13 +6351,13 @@
         <v>1</v>
       </c>
       <c r="F230">
-        <v>4989.666680987662</v>
+        <v>4988.00001489223</v>
       </c>
       <c r="G230">
-        <v>13668.50004486301</v>
+        <v>13668.16671164392</v>
       </c>
       <c r="H230">
-        <v>323446.9418874517</v>
+        <v>324620.9414850731</v>
       </c>
     </row>
     <row r="231">
@@ -6377,13 +6377,13 @@
         <v>1</v>
       </c>
       <c r="F231">
-        <v>4989.666636613311</v>
+        <v>4987.999968946278</v>
       </c>
       <c r="G231">
-        <v>13668.49998533076</v>
+        <v>13668.16665179735</v>
       </c>
       <c r="H231">
-        <v>323446.94586462</v>
+        <v>324620.9465692784</v>
       </c>
     </row>
     <row r="232">
@@ -6403,13 +6403,13 @@
         <v>1</v>
       </c>
       <c r="F232">
-        <v>4989.666681928573</v>
+        <v>4988.000015738405</v>
       </c>
       <c r="G232">
-        <v>13668.49999482516</v>
+        <v>13668.16666158712</v>
       </c>
       <c r="H232">
-        <v>323446.9443499917</v>
+        <v>324620.9440143455</v>
       </c>
     </row>
     <row r="233">
@@ -6429,13 +6429,13 @@
         <v>1</v>
       </c>
       <c r="F233">
-        <v>4989.666666509848</v>
+        <v>4987.999999858971</v>
       </c>
       <c r="G233">
-        <v>13668.50000833964</v>
+        <v>13668.16667500947</v>
       </c>
       <c r="H233">
-        <v>323446.9440340211</v>
+        <v>324620.944022899</v>
       </c>
     </row>
     <row r="234">
@@ -6455,13 +6455,13 @@
         <v>1</v>
       </c>
       <c r="F234">
-        <v>4989.666661683911</v>
+        <v>4987.999994847884</v>
       </c>
       <c r="G234">
-        <v>13668.49999616519</v>
+        <v>13668.16666279798</v>
       </c>
       <c r="H234">
-        <v>323446.9447495443</v>
+        <v>324620.944868841</v>
       </c>
     </row>
     <row r="235">
@@ -6481,13 +6481,13 @@
         <v>1</v>
       </c>
       <c r="F235">
-        <v>4989.666670040778</v>
+        <v>4988.000003481753</v>
       </c>
       <c r="G235">
-        <v>13668.49999977666</v>
+        <v>13668.16666646486</v>
       </c>
       <c r="H235">
-        <v>323446.9443778524</v>
+        <v>324620.9443020285</v>
       </c>
     </row>
     <row r="236">
@@ -6507,13 +6507,13 @@
         <v>1</v>
       </c>
       <c r="F236">
-        <v>4989.666666078179</v>
+        <v>4987.999999396203</v>
       </c>
       <c r="G236">
-        <v>13668.50000142717</v>
+        <v>13668.16666809077</v>
       </c>
       <c r="H236">
-        <v>323446.9443871392</v>
+        <v>324620.9443979228</v>
       </c>
     </row>
     <row r="237">
@@ -6533,13 +6533,13 @@
         <v>1</v>
       </c>
       <c r="F237">
-        <v>4989.666665934289</v>
+        <v>4987.999999241947</v>
       </c>
       <c r="G237">
-        <v>13668.49999912301</v>
+        <v>13668.16666578453</v>
       </c>
       <c r="H237">
-        <v>323446.9445048453</v>
+        <v>324620.9445229308</v>
       </c>
     </row>
     <row r="238">
@@ -6559,13 +6559,13 @@
         <v>1</v>
       </c>
       <c r="F238">
-        <v>4989.666667351082</v>
+        <v>4988.000000706635</v>
       </c>
       <c r="G238">
-        <v>13668.50000010895</v>
+        <v>13668.16666678005</v>
       </c>
       <c r="H238">
-        <v>323446.944423279</v>
+        <v>324620.9444076274</v>
       </c>
     </row>
     <row r="239">
@@ -6585,13 +6585,13 @@
         <v>1</v>
       </c>
       <c r="F239">
-        <v>4989.666666454516</v>
+        <v>4987.999999781595</v>
       </c>
       <c r="G239">
-        <v>13668.50000021971</v>
+        <v>13668.16666688512</v>
       </c>
       <c r="H239">
-        <v>323446.9444384212</v>
+        <v>324620.944442827</v>
       </c>
     </row>
     <row r="240">
@@ -6611,13 +6611,13 @@
         <v>1</v>
       </c>
       <c r="F240">
-        <v>4989.666666579962</v>
+        <v>4987.999999910059</v>
       </c>
       <c r="G240">
-        <v>13668.49999981722</v>
+        <v>13668.16666648324</v>
       </c>
       <c r="H240">
-        <v>323446.9444555151</v>
+        <v>324620.9444577951</v>
       </c>
     </row>
     <row r="241">
@@ -6637,13 +6637,13 @@
         <v>1</v>
       </c>
       <c r="F241">
-        <v>4989.666666795187</v>
+        <v>4988.000000132763</v>
       </c>
       <c r="G241">
-        <v>13668.50000004862</v>
+        <v>13668.16666671614</v>
       </c>
       <c r="H241">
-        <v>323446.9444390718</v>
+        <v>324620.9444360831</v>
       </c>
     </row>
     <row r="242">
@@ -6663,13 +6663,13 @@
         <v>1</v>
       </c>
       <c r="F242">
-        <v>4989.666666609888</v>
+        <v>4987.999999941472</v>
       </c>
       <c r="G242">
-        <v>13668.50000002852</v>
+        <v>13668.16666669483</v>
       </c>
       <c r="H242">
-        <v>323446.944444336</v>
+        <v>324620.9444455684</v>
       </c>
     </row>
     <row r="243">
@@ -6689,13 +6689,13 @@
         <v>1</v>
       </c>
       <c r="F243">
-        <v>4989.666666661679</v>
+        <v>4987.999999994765</v>
       </c>
       <c r="G243">
-        <v>13668.49999996479</v>
+        <v>13668.1666666314</v>
       </c>
       <c r="H243">
-        <v>323446.9444463076</v>
+        <v>324620.9444464822</v>
       </c>
     </row>
     <row r="244">
@@ -6715,13 +6715,13 @@
         <v>1</v>
       </c>
       <c r="F244">
-        <v>4989.666666688918</v>
+        <v>4988.000000023</v>
       </c>
       <c r="G244">
-        <v>13668.50000001398</v>
+        <v>13668.16666668079</v>
       </c>
       <c r="H244">
-        <v>323446.9444432384</v>
+        <v>324620.9444427113</v>
       </c>
     </row>
     <row r="245">
@@ -6741,13 +6741,13 @@
         <v>1</v>
       </c>
       <c r="F245">
-        <v>4989.666666653495</v>
+        <v>4987.999999986412</v>
       </c>
       <c r="G245">
-        <v>13668.50000000243</v>
+        <v>13668.16666666901</v>
       </c>
       <c r="H245">
-        <v>323446.9444446273</v>
+        <v>324620.9444449206</v>
       </c>
     </row>
     <row r="246">
@@ -6767,13 +6767,13 @@
         <v>1</v>
       </c>
       <c r="F246">
-        <v>4989.66666666803</v>
+        <v>4988.000000001392</v>
       </c>
       <c r="G246">
-        <v>13668.49999999373</v>
+        <v>13668.1666666604</v>
       </c>
       <c r="H246">
-        <v>323446.9444447245</v>
+        <v>324620.9444447047</v>
       </c>
     </row>
     <row r="247">
@@ -6793,13 +6793,13 @@
         <v>1</v>
       </c>
       <c r="F247">
-        <v>4989.666666670148</v>
+        <v>4988.000000003602</v>
       </c>
       <c r="G247">
-        <v>13668.50000000338</v>
+        <v>13668.16666667006</v>
       </c>
       <c r="H247">
-        <v>323446.9444441968</v>
+        <v>324620.9444441122</v>
       </c>
     </row>
     <row r="248">
@@ -6819,13 +6819,13 @@
         <v>1</v>
       </c>
       <c r="F248">
-        <v>4989.666666663891</v>
+        <v>4987.999999997135</v>
       </c>
       <c r="G248">
-        <v>13668.49999999985</v>
+        <v>13668.16666666649</v>
       </c>
       <c r="H248">
-        <v>323446.9444445162</v>
+        <v>324620.9444445792</v>
       </c>
     </row>
     <row r="249">
@@ -6845,13 +6845,13 @@
         <v>1</v>
       </c>
       <c r="F249">
-        <v>4989.666666667356</v>
+        <v>4988.000000000709</v>
       </c>
       <c r="G249">
-        <v>13668.49999999899</v>
+        <v>13668.16666666565</v>
       </c>
       <c r="H249">
-        <v>323446.9444444791</v>
+        <v>324620.9444444653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q1 advanced estimate data update
</commit_message>
<xml_diff>
--- a/data/raw/haver/economic_statistics.xlsx
+++ b/data/raw/haver/economic_statistics.xlsx
@@ -5707,7 +5707,7 @@
         <v>13655.33333333333</v>
       </c>
       <c r="H205">
-        <v>327589.6666666667</v>
+        <v>327773.6666666667</v>
       </c>
     </row>
     <row r="206">
@@ -5715,7 +5715,7 @@
         <v>44286</v>
       </c>
       <c r="B206">
-        <v>252.4233333333333</v>
+        <v>257.3506666666667</v>
       </c>
       <c r="C206">
         <v>19502.8</v>
@@ -5727,13 +5727,13 @@
         <v>1</v>
       </c>
       <c r="F206">
-        <v>5007</v>
+        <v>4988.666666666667</v>
       </c>
       <c r="G206">
-        <v>13653.88888888889</v>
+        <v>13686</v>
       </c>
       <c r="H206">
-        <v>324519.3333333333</v>
+        <v>324580.6666666667</v>
       </c>
     </row>
     <row r="207">
@@ -5741,7 +5741,7 @@
         <v>44377</v>
       </c>
       <c r="B207">
-        <v>253.3724444444444</v>
+        <v>255.0148888888889</v>
       </c>
       <c r="C207">
         <v>19594.2</v>
@@ -5753,13 +5753,13 @@
         <v>1</v>
       </c>
       <c r="F207">
-        <v>4992.888888888889</v>
+        <v>4986.777777777777</v>
       </c>
       <c r="G207">
-        <v>13681.96296296296</v>
+        <v>13692.66666666667</v>
       </c>
       <c r="H207">
-        <v>323699.1111111111</v>
+        <v>323780.8888888889</v>
       </c>
     </row>
     <row r="208">
@@ -5767,7 +5767,7 @@
         <v>44469</v>
       </c>
       <c r="B208">
-        <v>253.492037037037</v>
+        <v>255.681962962963</v>
       </c>
       <c r="C208">
         <v>19687.7</v>
@@ -5779,13 +5779,13 @@
         <v>1</v>
       </c>
       <c r="F208">
-        <v>4978.407407407407</v>
+        <v>4970.259259259259</v>
       </c>
       <c r="G208">
-        <v>13663.72839506173</v>
+        <v>13678</v>
       </c>
       <c r="H208">
-        <v>325269.3703703704</v>
+        <v>325378.4074074074</v>
       </c>
     </row>
     <row r="209">
@@ -5793,7 +5793,7 @@
         <v>44561</v>
       </c>
       <c r="B209">
-        <v>253.0959382716049</v>
+        <v>256.0158395061728</v>
       </c>
       <c r="C209">
         <v>19783.1</v>
@@ -5805,13 +5805,13 @@
         <v>1</v>
       </c>
       <c r="F209">
-        <v>4992.765432098765</v>
+        <v>4981.901234567901</v>
       </c>
       <c r="G209">
-        <v>13666.52674897119</v>
+        <v>13685.55555555556</v>
       </c>
       <c r="H209">
-        <v>324495.9382716049</v>
+        <v>324579.987654321</v>
       </c>
     </row>
     <row r="210">
@@ -5819,7 +5819,7 @@
         <v>44651</v>
       </c>
       <c r="B210">
-        <v>253.3201399176955</v>
+        <v>255.5708971193415</v>
       </c>
       <c r="C210">
         <v>19879.6</v>
@@ -5831,13 +5831,13 @@
         <v>1</v>
       </c>
       <c r="F210">
-        <v>4988.020576131687</v>
+        <v>4979.64609053498</v>
       </c>
       <c r="G210">
-        <v>13670.73936899863</v>
+        <v>13685.40740740741</v>
       </c>
       <c r="H210">
-        <v>324488.1399176955</v>
+        <v>324579.7613168724</v>
       </c>
     </row>
     <row r="211">
@@ -5845,7 +5845,7 @@
         <v>44742</v>
       </c>
       <c r="B211">
-        <v>253.3027050754458</v>
+        <v>255.7562331961591</v>
       </c>
       <c r="C211">
         <v>19975.5</v>
@@ -5857,13 +5857,13 @@
         <v>1</v>
       </c>
       <c r="F211">
-        <v>4986.39780521262</v>
+        <v>4977.268861454047</v>
       </c>
       <c r="G211">
-        <v>13666.99817101052</v>
+        <v>13682.98765432099</v>
       </c>
       <c r="H211">
-        <v>324751.1495198903</v>
+        <v>324846.0521262003</v>
       </c>
     </row>
     <row r="212">
@@ -5871,7 +5871,7 @@
         <v>44834</v>
       </c>
       <c r="B212">
-        <v>253.2395944215821</v>
+        <v>255.7809899405578</v>
       </c>
       <c r="C212">
         <v>20069.9</v>
@@ -5883,13 +5883,13 @@
         <v>1</v>
       </c>
       <c r="F212">
-        <v>4989.061271147691</v>
+        <v>4979.605395518976</v>
       </c>
       <c r="G212">
-        <v>13668.08809632678</v>
+        <v>13684.65020576132</v>
       </c>
       <c r="H212">
-        <v>324578.4092363969</v>
+        <v>324668.6003657979</v>
       </c>
     </row>
     <row r="213">
@@ -5897,7 +5897,7 @@
         <v>44926</v>
       </c>
       <c r="B213">
-        <v>253.2874798049078</v>
+        <v>255.7027067520195</v>
       </c>
       <c r="C213">
         <v>20163.7</v>
@@ -5909,13 +5909,13 @@
         <v>1</v>
       </c>
       <c r="F213">
-        <v>4987.826550830666</v>
+        <v>4978.840115836</v>
       </c>
       <c r="G213">
-        <v>13668.60854544531</v>
+        <v>13684.34842249657</v>
       </c>
       <c r="H213">
-        <v>324605.8995579942</v>
+        <v>324698.1379362902</v>
       </c>
     </row>
     <row r="214">
@@ -5923,7 +5923,7 @@
         <v>45016</v>
       </c>
       <c r="B214">
-        <v>253.2765931006452</v>
+        <v>255.7466432962455</v>
       </c>
       <c r="C214">
         <v>20257.3</v>
@@ -5935,13 +5935,13 @@
         <v>1</v>
       </c>
       <c r="F214">
-        <v>4987.761875730325</v>
+        <v>4978.571457603008</v>
       </c>
       <c r="G214">
-        <v>13667.89827092754</v>
+        <v>13683.99542752629</v>
       </c>
       <c r="H214">
-        <v>324645.1527714271</v>
+        <v>324737.5968094295</v>
       </c>
     </row>
     <row r="215">
@@ -5949,7 +5949,7 @@
         <v>45107</v>
       </c>
       <c r="B215">
-        <v>253.267889109045</v>
+        <v>255.7434466629409</v>
       </c>
       <c r="C215">
         <v>20351.2</v>
@@ -5961,13 +5961,13 @@
         <v>1</v>
       </c>
       <c r="F215">
-        <v>4988.216565902894</v>
+        <v>4979.005656319328</v>
       </c>
       <c r="G215">
-        <v>13668.19830423321</v>
+        <v>13684.33135192806</v>
       </c>
       <c r="H215">
-        <v>324609.8205219394</v>
+        <v>324701.4450371725</v>
       </c>
     </row>
     <row r="216">
@@ -5975,7 +5975,7 @@
         <v>45199</v>
       </c>
       <c r="B216">
-        <v>253.2773206715327</v>
+        <v>255.7309322370686</v>
       </c>
       <c r="C216">
         <v>20446</v>
@@ -5987,13 +5987,13 @@
         <v>1</v>
       </c>
       <c r="F216">
-        <v>4987.934997487962</v>
+        <v>4978.805743252779</v>
       </c>
       <c r="G216">
-        <v>13668.23504020202</v>
+        <v>13684.22506731698</v>
       </c>
       <c r="H216">
-        <v>324620.2909504536</v>
+        <v>324712.3932609641</v>
       </c>
     </row>
     <row r="217">
@@ -6001,7 +6001,7 @@
         <v>45291</v>
       </c>
       <c r="B217">
-        <v>253.273934293741</v>
+        <v>255.740340732085</v>
       </c>
       <c r="C217">
         <v>20541.7</v>
@@ -6013,13 +6013,13 @@
         <v>1</v>
       </c>
       <c r="F217">
-        <v>4987.971146373727</v>
+        <v>4978.794285725038</v>
       </c>
       <c r="G217">
-        <v>13668.11053845425</v>
+        <v>13684.18394892378</v>
       </c>
       <c r="H217">
-        <v>324625.0880812734</v>
+        <v>324717.1450358554</v>
       </c>
     </row>
     <row r="218">
@@ -6027,7 +6027,7 @@
         <v>45382</v>
       </c>
       <c r="B218">
-        <v>253.2730480247729</v>
+        <v>255.7382398773649</v>
       </c>
       <c r="C218">
         <v>20638</v>
@@ -6039,13 +6039,13 @@
         <v>1</v>
       </c>
       <c r="F218">
-        <v>4988.040903254861</v>
+        <v>4978.868561765715</v>
       </c>
       <c r="G218">
-        <v>13668.18129429649</v>
+        <v>13684.2467893896</v>
       </c>
       <c r="H218">
-        <v>324618.3998512221</v>
+        <v>324710.3277779973</v>
       </c>
     </row>
     <row r="219">
@@ -6053,7 +6053,7 @@
         <v>45473</v>
       </c>
       <c r="B219">
-        <v>253.2747676633489</v>
+        <v>255.7365042821728</v>
       </c>
       <c r="C219">
         <v>20734.1</v>
@@ -6065,13 +6065,13 @@
         <v>1</v>
       </c>
       <c r="F219">
-        <v>4987.98234903885</v>
+        <v>4978.822863581177</v>
       </c>
       <c r="G219">
-        <v>13668.17562431759</v>
+        <v>13684.21860187678</v>
       </c>
       <c r="H219">
-        <v>324621.2596276497</v>
+        <v>324713.2886916056</v>
       </c>
     </row>
     <row r="220">
@@ -6079,7 +6079,7 @@
         <v>45565</v>
       </c>
       <c r="B220">
-        <v>253.2739166606209</v>
+        <v>255.7383616305409</v>
       </c>
       <c r="C220">
         <v>20830.5</v>
@@ -6091,13 +6091,13 @@
         <v>1</v>
       </c>
       <c r="F220">
-        <v>4987.998132889145</v>
+        <v>4978.82857035731</v>
       </c>
       <c r="G220">
-        <v>13668.15581902278</v>
+        <v>13684.21644673005</v>
       </c>
       <c r="H220">
-        <v>324621.5825200484</v>
+        <v>324713.5871684861</v>
       </c>
     </row>
     <row r="221">
@@ -6105,7 +6105,7 @@
         <v>45657</v>
       </c>
       <c r="B221">
-        <v>253.2739107829142</v>
+        <v>255.7377019300262</v>
       </c>
       <c r="C221">
         <v>20927.1</v>
@@ -6117,13 +6117,13 @@
         <v>1</v>
       </c>
       <c r="F221">
-        <v>4988.007128394285</v>
+        <v>4978.839998568067</v>
       </c>
       <c r="G221">
-        <v>13668.17091254562</v>
+        <v>13684.22727933215</v>
       </c>
       <c r="H221">
-        <v>324620.41399964</v>
+        <v>324712.4012126963</v>
       </c>
     </row>
     <row r="222">
@@ -6131,7 +6131,7 @@
         <v>45747</v>
       </c>
       <c r="B222">
-        <v>253.2741983689613</v>
+        <v>255.7375226142466</v>
       </c>
       <c r="C222">
         <v>21023.6</v>
@@ -6143,13 +6143,13 @@
         <v>1</v>
       </c>
       <c r="F222">
-        <v>4987.995870107427</v>
+        <v>4978.830477502185</v>
       </c>
       <c r="G222">
-        <v>13668.16745196199</v>
+        <v>13684.22077597966</v>
       </c>
       <c r="H222">
-        <v>324621.085382446</v>
+        <v>324713.092357596</v>
       </c>
     </row>
     <row r="223">
@@ -6157,7 +6157,7 @@
         <v>45838</v>
       </c>
       <c r="B223">
-        <v>253.2740086041655</v>
+        <v>255.7378620582713</v>
       </c>
       <c r="C223">
         <v>21118.9</v>
@@ -6169,13 +6169,13 @@
         <v>1</v>
       </c>
       <c r="F223">
-        <v>4988.000377130285</v>
+        <v>4978.833015475854</v>
       </c>
       <c r="G223">
-        <v>13668.16472784346</v>
+        <v>13684.22150068062</v>
       </c>
       <c r="H223">
-        <v>324621.0273007115</v>
+        <v>324713.0269129261</v>
       </c>
     </row>
     <row r="224">
@@ -6183,7 +6183,7 @@
         <v>45930</v>
       </c>
       <c r="B224">
-        <v>253.2740392520137</v>
+        <v>255.7376955341814</v>
       </c>
       <c r="C224">
         <v>21213.5</v>
@@ -6195,13 +6195,13 @@
         <v>1</v>
       </c>
       <c r="F224">
-        <v>4988.001125210666</v>
+        <v>4978.834497182035</v>
       </c>
       <c r="G224">
-        <v>13668.16769745036</v>
+        <v>13684.22318533081</v>
       </c>
       <c r="H224">
-        <v>324620.8422275992</v>
+        <v>324712.8401610728</v>
       </c>
     </row>
     <row r="225">
@@ -6209,7 +6209,7 @@
         <v>46022</v>
       </c>
       <c r="B225">
-        <v>253.2740820750468</v>
+        <v>255.7376934022331</v>
       </c>
       <c r="C225">
         <v>21307.4</v>
@@ -6221,13 +6221,13 @@
         <v>1</v>
       </c>
       <c r="F225">
-        <v>4987.999124149459</v>
+        <v>4978.832663386692</v>
       </c>
       <c r="G225">
-        <v>13668.16662575194</v>
+        <v>13684.2218206637</v>
       </c>
       <c r="H225">
-        <v>324620.9849702522</v>
+        <v>324712.9864771983</v>
       </c>
     </row>
     <row r="226">
@@ -6235,7 +6235,7 @@
         <v>46112</v>
       </c>
       <c r="B226">
-        <v>253.2740433104087</v>
+        <v>255.7377503315619</v>
       </c>
       <c r="C226">
         <v>21400.7</v>
@@ -6247,13 +6247,13 @@
         <v>1</v>
       </c>
       <c r="F226">
-        <v>4988.000208830137</v>
+        <v>4978.833392014861</v>
       </c>
       <c r="G226">
-        <v>13668.16635034859</v>
+        <v>13684.22216889171</v>
       </c>
       <c r="H226">
-        <v>324620.951499521</v>
+        <v>324712.9511837324</v>
       </c>
     </row>
     <row r="227">
@@ -6261,7 +6261,7 @@
         <v>46203</v>
       </c>
       <c r="B227">
-        <v>253.2740548791564</v>
+        <v>255.7377130893254</v>
       </c>
       <c r="C227">
         <v>21493.1</v>
@@ -6273,13 +6273,13 @@
         <v>1</v>
       </c>
       <c r="F227">
-        <v>4988.000152730087</v>
+        <v>4978.833517527863</v>
       </c>
       <c r="G227">
-        <v>13668.16689118363</v>
+        <v>13684.22239162874</v>
       </c>
       <c r="H227">
-        <v>324620.9262324575</v>
+        <v>324712.9259406679</v>
       </c>
     </row>
     <row r="228">
@@ -6287,7 +6287,7 @@
         <v>46295</v>
       </c>
       <c r="B228">
-        <v>253.274060088204</v>
+        <v>255.7377189410401</v>
       </c>
       <c r="C228">
         <v>21585.4</v>
@@ -6299,13 +6299,13 @@
         <v>1</v>
       </c>
       <c r="F228">
-        <v>4987.999828569895</v>
+        <v>4978.833190976472</v>
       </c>
       <c r="G228">
-        <v>13668.16662242805</v>
+        <v>13684.22212706138</v>
       </c>
       <c r="H228">
-        <v>324620.9542340769</v>
+        <v>324712.9545338662</v>
       </c>
     </row>
     <row r="229">
@@ -6313,7 +6313,7 @@
         <v>46387</v>
       </c>
       <c r="B229">
-        <v>253.2740527592563</v>
+        <v>255.7377274539758</v>
       </c>
       <c r="C229">
         <v>21677.8</v>
@@ -6325,13 +6325,13 @@
         <v>1</v>
       </c>
       <c r="F229">
-        <v>4988.000063376707</v>
+        <v>4978.833366839732</v>
       </c>
       <c r="G229">
-        <v>13668.16662132009</v>
+        <v>13684.22222919394</v>
       </c>
       <c r="H229">
-        <v>324620.9439886851</v>
+        <v>324712.9438860889</v>
       </c>
     </row>
     <row r="230">
@@ -6339,7 +6339,7 @@
         <v>46477</v>
       </c>
       <c r="B230">
-        <v>253.2740559088722</v>
+        <v>255.7377198281138</v>
       </c>
       <c r="C230">
         <v>21770.3</v>
@@ -6351,13 +6351,13 @@
         <v>1</v>
       </c>
       <c r="F230">
-        <v>4988.00001489223</v>
+        <v>4978.833358448022</v>
       </c>
       <c r="G230">
-        <v>13668.16671164392</v>
+        <v>13684.22224929469</v>
       </c>
       <c r="H230">
-        <v>324620.9414850731</v>
+        <v>324712.941453541</v>
       </c>
     </row>
     <row r="231">
@@ -6365,7 +6365,7 @@
         <v>46568</v>
       </c>
       <c r="B231">
-        <v>253.2740562521108</v>
+        <v>255.7377220743766</v>
       </c>
       <c r="C231">
         <v>21862.9</v>
@@ -6377,13 +6377,13 @@
         <v>1</v>
       </c>
       <c r="F231">
-        <v>4987.999968946278</v>
+        <v>4978.833305421409</v>
       </c>
       <c r="G231">
-        <v>13668.16665179735</v>
+        <v>13684.22220185</v>
       </c>
       <c r="H231">
-        <v>324620.9465692784</v>
+        <v>324712.9466244987</v>
       </c>
     </row>
     <row r="232">
@@ -6391,7 +6391,7 @@
         <v>46660</v>
       </c>
       <c r="B232">
-        <v>253.2740549734131</v>
+        <v>255.7377231188221</v>
       </c>
       <c r="C232">
         <v>21956.1</v>
@@ -6403,13 +6403,13 @@
         <v>1</v>
       </c>
       <c r="F232">
-        <v>4988.000015738405</v>
+        <v>4978.833343569721</v>
       </c>
       <c r="G232">
-        <v>13668.16666158712</v>
+        <v>13684.22222677954</v>
       </c>
       <c r="H232">
-        <v>324620.9440143455</v>
+        <v>324712.9439880428</v>
       </c>
     </row>
     <row r="233">
@@ -6417,7 +6417,7 @@
         <v>46752</v>
       </c>
       <c r="B233">
-        <v>253.2740557114654</v>
+        <v>255.7377216737708</v>
       </c>
       <c r="C233">
         <v>22049.5</v>
@@ -6429,13 +6429,13 @@
         <v>1</v>
       </c>
       <c r="F233">
-        <v>4987.999999858971</v>
+        <v>4978.833335813051</v>
       </c>
       <c r="G233">
-        <v>13668.16667500947</v>
+        <v>13684.22222597475</v>
       </c>
       <c r="H233">
-        <v>324620.944022899</v>
+        <v>324712.9440220275</v>
       </c>
     </row>
     <row r="234">
@@ -6443,7 +6443,7 @@
         <v>46843</v>
       </c>
       <c r="B234">
-        <v>253.2740556456631</v>
+        <v>255.7377222889898</v>
       </c>
       <c r="C234">
         <v>22143.3</v>
@@ -6455,13 +6455,13 @@
         <v>1</v>
       </c>
       <c r="F234">
-        <v>4987.999994847884</v>
+        <v>4978.833328268061</v>
       </c>
       <c r="G234">
-        <v>13668.16666279798</v>
+        <v>13684.22221820143</v>
       </c>
       <c r="H234">
-        <v>324620.944868841</v>
+        <v>324712.9448781897</v>
       </c>
     </row>
     <row r="235">
@@ -6469,7 +6469,7 @@
         <v>46934</v>
       </c>
       <c r="B235">
-        <v>253.2740554435139</v>
+        <v>255.7377223605276</v>
       </c>
       <c r="C235">
         <v>22238.3</v>
@@ -6481,13 +6481,13 @@
         <v>1</v>
       </c>
       <c r="F235">
-        <v>4988.000003481753</v>
+        <v>4978.833335883611</v>
       </c>
       <c r="G235">
-        <v>13668.16666646486</v>
+        <v>13684.22222365191</v>
       </c>
       <c r="H235">
-        <v>324620.9443020285</v>
+        <v>324712.9442960867</v>
       </c>
     </row>
     <row r="236">
@@ -6495,7 +6495,7 @@
         <v>47026</v>
       </c>
       <c r="B236">
-        <v>253.2740556002141</v>
+        <v>255.7377221077627</v>
       </c>
       <c r="C236">
         <v>22334.3</v>
@@ -6507,13 +6507,13 @@
         <v>1</v>
       </c>
       <c r="F236">
-        <v>4987.999999396203</v>
+        <v>4978.833333321574</v>
       </c>
       <c r="G236">
-        <v>13668.16666809077</v>
+        <v>13684.22222260936</v>
       </c>
       <c r="H236">
-        <v>324620.9443979228</v>
+        <v>324712.944398768</v>
       </c>
     </row>
     <row r="237">
@@ -6521,7 +6521,7 @@
         <v>47118</v>
       </c>
       <c r="B237">
-        <v>253.2740555631304</v>
+        <v>255.7377222524267</v>
       </c>
       <c r="C237">
         <v>22431.4</v>
@@ -6533,13 +6533,13 @@
         <v>1</v>
       </c>
       <c r="F237">
-        <v>4987.999999241947</v>
+        <v>4978.833332491082</v>
       </c>
       <c r="G237">
-        <v>13668.16666578453</v>
+        <v>13684.22222148757</v>
       </c>
       <c r="H237">
-        <v>324620.9445229308</v>
+        <v>324712.9445243481</v>
       </c>
     </row>
     <row r="238">
@@ -6547,7 +6547,7 @@
         <v>47208</v>
       </c>
       <c r="B238">
-        <v>253.2740555356195</v>
+        <v>255.737722240239</v>
       </c>
       <c r="C238">
         <v>22529.4</v>
@@ -6559,13 +6559,13 @@
         <v>1</v>
       </c>
       <c r="F238">
-        <v>4988.000000706635</v>
+        <v>4978.833333898756</v>
       </c>
       <c r="G238">
-        <v>13668.16666678005</v>
+        <v>13684.22222258295</v>
       </c>
       <c r="H238">
-        <v>324620.9444076274</v>
+        <v>324712.9444064009</v>
       </c>
     </row>
     <row r="239">
@@ -6573,7 +6573,7 @@
         <v>47299</v>
       </c>
       <c r="B239">
-        <v>253.2740555663213</v>
+        <v>255.7377222001428</v>
       </c>
       <c r="C239">
         <v>22628.1</v>
@@ -6585,13 +6585,13 @@
         <v>1</v>
       </c>
       <c r="F239">
-        <v>4987.999999781595</v>
+        <v>4978.833333237138</v>
       </c>
       <c r="G239">
-        <v>13668.16666688512</v>
+        <v>13684.22222222662</v>
       </c>
       <c r="H239">
-        <v>324620.944442827</v>
+        <v>324712.9444431723</v>
       </c>
     </row>
     <row r="240">
@@ -6599,7 +6599,7 @@
         <v>47391</v>
       </c>
       <c r="B240">
-        <v>253.2740555550237</v>
+        <v>255.7377222309362</v>
       </c>
       <c r="C240">
         <v>22726.7</v>
@@ -6611,13 +6611,13 @@
         <v>1</v>
       </c>
       <c r="F240">
-        <v>4987.999999910059</v>
+        <v>4978.833333208992</v>
       </c>
       <c r="G240">
-        <v>13668.16666648324</v>
+        <v>13684.22222209904</v>
       </c>
       <c r="H240">
-        <v>324620.9444577951</v>
+        <v>324712.9444579738</v>
       </c>
     </row>
     <row r="241">
@@ -6625,7 +6625,7 @@
         <v>47483</v>
       </c>
       <c r="B241">
-        <v>253.2740555523215</v>
+        <v>255.7377222237726</v>
       </c>
       <c r="C241">
         <v>22825.1</v>
@@ -6637,13 +6637,13 @@
         <v>1</v>
       </c>
       <c r="F241">
-        <v>4988.000000132763</v>
+        <v>4978.833333448295</v>
       </c>
       <c r="G241">
-        <v>13668.16666671614</v>
+        <v>13684.22222230287</v>
       </c>
       <c r="H241">
-        <v>324620.9444360831</v>
+        <v>324712.944435849</v>
       </c>
     </row>
     <row r="242">
@@ -6651,7 +6651,7 @@
         <v>47573</v>
       </c>
       <c r="B242">
-        <v>253.2740555578889</v>
+        <v>255.7377222182839</v>
       </c>
       <c r="C242">
         <v>22923.6</v>
@@ -6663,13 +6663,13 @@
         <v>1</v>
       </c>
       <c r="F242">
-        <v>4987.999999941472</v>
+        <v>4978.833333298141</v>
       </c>
       <c r="G242">
-        <v>13668.16666669483</v>
+        <v>13684.22222220951</v>
       </c>
       <c r="H242">
-        <v>324620.9444455684</v>
+        <v>324712.944445665</v>
       </c>
     </row>
     <row r="243">
@@ -6677,7 +6677,7 @@
         <v>47664</v>
       </c>
       <c r="B243">
-        <v>253.274055555078</v>
+        <v>255.7377222243309</v>
       </c>
       <c r="C243">
         <v>23022.1</v>
@@ -6689,13 +6689,13 @@
         <v>1</v>
       </c>
       <c r="F243">
-        <v>4987.999999994765</v>
+        <v>4978.833333318476</v>
       </c>
       <c r="G243">
-        <v>13668.1666666314</v>
+        <v>13684.22222220381</v>
       </c>
       <c r="H243">
-        <v>324620.9444464822</v>
+        <v>324712.9444464959</v>
       </c>
     </row>
     <row r="244">
@@ -6703,7 +6703,7 @@
         <v>47756</v>
       </c>
       <c r="B244">
-        <v>253.2740555550961</v>
+        <v>255.7377222221291</v>
       </c>
       <c r="C244">
         <v>23120.6</v>
@@ -6715,13 +6715,13 @@
         <v>1</v>
       </c>
       <c r="F244">
-        <v>4988.000000023</v>
+        <v>4978.833333354971</v>
       </c>
       <c r="G244">
-        <v>13668.16666668079</v>
+        <v>13684.22222223873</v>
       </c>
       <c r="H244">
-        <v>324620.9444427113</v>
+        <v>324712.94444267</v>
       </c>
     </row>
     <row r="245">
@@ -6729,7 +6729,7 @@
         <v>47848</v>
       </c>
       <c r="B245">
-        <v>253.274055556021</v>
+        <v>255.7377222215813</v>
       </c>
       <c r="C245">
         <v>23219.4</v>
@@ -6741,13 +6741,13 @@
         <v>1</v>
       </c>
       <c r="F245">
-        <v>4987.999999986412</v>
+        <v>4978.833333323863</v>
       </c>
       <c r="G245">
-        <v>13668.16666666901</v>
+        <v>13684.22222221735</v>
       </c>
       <c r="H245">
-        <v>324620.9444449206</v>
+        <v>324712.9444449436</v>
       </c>
     </row>
     <row r="246">
@@ -6755,7 +6755,7 @@
         <v>47938</v>
       </c>
       <c r="B246">
-        <v>253.2740555553984</v>
+        <v>255.7377222226805</v>
       </c>
       <c r="C246">
         <v>23318.3</v>
@@ -6767,13 +6767,13 @@
         <v>1</v>
       </c>
       <c r="F246">
-        <v>4988.000000001392</v>
+        <v>4978.833333332436</v>
       </c>
       <c r="G246">
-        <v>13668.1666666604</v>
+        <v>13684.22222221996</v>
       </c>
       <c r="H246">
-        <v>324620.9444447047</v>
+        <v>324712.9444447032</v>
       </c>
     </row>
     <row r="247">
@@ -6781,7 +6781,7 @@
         <v>48029</v>
       </c>
       <c r="B247">
-        <v>253.2740555555052</v>
+        <v>255.7377222221303</v>
       </c>
       <c r="C247">
         <v>23417.4</v>
@@ -6793,13 +6793,13 @@
         <v>1</v>
       </c>
       <c r="F247">
-        <v>4988.000000003602</v>
+        <v>4978.83333333709</v>
       </c>
       <c r="G247">
-        <v>13668.16666667006</v>
+        <v>13684.22222222535</v>
       </c>
       <c r="H247">
-        <v>324620.9444441122</v>
+        <v>324712.9444441056</v>
       </c>
     </row>
     <row r="248">
@@ -6807,7 +6807,7 @@
         <v>48121</v>
       </c>
       <c r="B248">
-        <v>253.2740555556415</v>
+        <v>255.7377222221307</v>
       </c>
       <c r="C248">
         <v>23516.4</v>
@@ -6819,13 +6819,13 @@
         <v>1</v>
       </c>
       <c r="F248">
-        <v>4987.999999997135</v>
+        <v>4978.833333331129</v>
       </c>
       <c r="G248">
-        <v>13668.16666666649</v>
+        <v>13684.22222222089</v>
       </c>
       <c r="H248">
-        <v>324620.9444445792</v>
+        <v>324712.9444445841</v>
       </c>
     </row>
     <row r="249">
@@ -6833,7 +6833,7 @@
         <v>48213</v>
       </c>
       <c r="B249">
-        <v>253.2740555555151</v>
+        <v>255.7377222223138</v>
       </c>
       <c r="C249">
         <v>23615.3</v>
@@ -6845,13 +6845,13 @@
         <v>1</v>
       </c>
       <c r="F249">
-        <v>4988.000000000709</v>
+        <v>4978.833333333552</v>
       </c>
       <c r="G249">
-        <v>13668.16666666565</v>
+        <v>13684.22222222207</v>
       </c>
       <c r="H249">
-        <v>324620.9444444653</v>
+        <v>324712.9444444643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>